<commit_message>
add excel username and massages
</commit_message>
<xml_diff>
--- a/project1.xlsx
+++ b/project1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,11 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>massage one account</t>
         </is>
       </c>
@@ -446,7 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hi</t>
+          <t>SabaMosaybie</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>hello</t>
         </is>
       </c>
     </row>
@@ -456,27 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hello</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Appel</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cookie</t>
+          <t>narges__pv310</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>my name is selenium py</t>
         </is>
       </c>
     </row>

</xml_diff>